<commit_message>
process health care spending
</commit_message>
<xml_diff>
--- a/data/raw/Health_Care.xlsx
+++ b/data/raw/Health_Care.xlsx
@@ -54,9 +54,15 @@
     <style:style style:name="ro5" style:family="table-row">
       <style:table-row-properties style:row-height="0.1917in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
+    <style:style style:name="ro6" style:family="table-row">
+      <style:table-row-properties style:row-height="0.178in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
+    <number:number-style style:name="N1">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1"/>
+    </number:number-style>
     <number:number-style style:name="N3">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
@@ -80,16 +86,6 @@
       <style:paragraph-properties fo:text-align="start" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial, Helvetica, Helv" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial, Helvetica, Helv" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
-      <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="start" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial, Helvetica, Helv" fo:font-size="10pt" fo:font-style="italic" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-name-complex="Arial, Helvetica, Helv" style:font-size-complex="10pt" style:font-style-complex="italic" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
-      <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial, Helvetica, Helv" fo:font-size="10pt" fo:font-style="italic" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-name-complex="Arial, Helvetica, Helv" style:font-size-complex="10pt" style:font-style-complex="italic" style:font-weight-complex="bold"/>
-    </style:style>
     <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
@@ -100,12 +96,12 @@
       <style:paragraph-properties fo:text-align="end" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="20pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="20pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="20pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N144">
+    <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N1">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="italic" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="italic" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce10" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Currency" style:data-style-name="N146">
+    <style:style style:name="ce10" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Currency" style:data-style-name="N142">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="end" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
@@ -120,30 +116,20 @@
       <style:paragraph-properties fo:text-align="end" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce13" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
-      <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="start" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="italic" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="italic" style:font-weight-complex="bold"/>
-    </style:style>
     <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="20pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="20pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="20pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N145">
+    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N148">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N145">
+    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N148">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
-    </style:style>
-    <style:style style:name="ce17" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
-      <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="italic" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="italic" style:font-weight-complex="bold"/>
     </style:style>
     <style:style style:name="ce18" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N0">
       <style:table-cell-properties fo:background-color="#ffffff" style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
@@ -6306,32 +6292,15 @@
           <table:table-cell table:number-columns-repeated="992"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
-            <text:p>
-              NOTE: Numbers may not add to totals shown because of rounding. 
-              <text:s/>
-              Percent changes are calculated from unrounded data.
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" table:number-columns-repeated="30"/>
-          <table:table-cell table:style-name="ce17"/>
-          <table:table-cell table:style-name="ce13" table:number-columns-repeated="992"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
-            <text:p>SOURCE: Centers for Medicare and Medicaid Services, Office of the Actuary, National Health Statistics Group.</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" table:number-columns-repeated="30"/>
-          <table:table-cell table:style-name="ce17"/>
-          <table:table-cell table:style-name="ce13" table:number-columns-repeated="992"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro4">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5" table:number-rows-repeated="1048510">
+        <table:table-row table:style-name="ro5" table:number-rows-repeated="1048511">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5">
+        <table:table-row table:style-name="ro6">
+          <table:table-cell table:number-columns-repeated="1024"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
       </table:table>
@@ -6345,11 +6314,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-02-06T21:21:55.729197995</meta:creation-date>
-    <dc:date>2025-02-06T21:22:09.146134468</dc:date>
-    <meta:editing-duration>PT14S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="1955" meta:object-count="0"/>
+    <dc:date>2025-02-06T23:01:38.480005328</dc:date>
+    <meta:editing-duration>PT8M2S</meta:editing-duration>
+    <meta:editing-cycles>3</meta:editing-cycles>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="1953" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -6361,14 +6330,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">87311</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">36689</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">35736</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">62</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -6427,9 +6396,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">oAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -6441,6 +6410,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="Sheet1">
@@ -6470,280 +6440,91 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:number-style style:name="N139P0" style:volatile="true">
+    <number:number-style style:name="N124P0" style:volatile="true">
       <number:text> $</number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N139P1" style:volatile="true">
+    <number:number-style style:name="N124P1" style:volatile="true">
       <number:text> $</number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
-    <number:number-style style:name="N139P2" style:volatile="true">
+    <number:number-style style:name="N124P2" style:volatile="true">
       <number:text> $</number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N139">
+    <number:text-style style:name="N124">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N139P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N139P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N139P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N124P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N124P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N124P2"/>
     </number:text-style>
-    <number:number-style style:name="N147">
-      <number:text>$</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-    </number:number-style>
-    <number:number-style style:name="N146P0" style:volatile="true">
-      <number:text> $</number:text>
-      <number:fill-character> </number:fill-character>
+    <number:number-style style:name="N164P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N146P1" style:volatile="true">
-      <number:text> $</number:text>
-      <number:fill-character> </number:fill-character>
+    <number:number-style style:name="N164">
+      <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N164P0"/>
     </number:number-style>
-    <number:number-style style:name="N146P2" style:volatile="true">
-      <number:text> $</number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+    <number:number-style style:name="N162P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N146">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N146P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N146P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N146P2"/>
-    </number:text-style>
-    <number:percentage-style style:name="N145">
-      <number:number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1"/>
-      <number:text>%</number:text>
-    </number:percentage-style>
-    <number:number-style style:name="N144">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1"/>
+    <number:number-style style:name="N162">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N162P0"/>
     </number:number-style>
-    <number:number-style style:name="N143">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
-    </number:number-style>
-    <number:time-style style:name="N142">
+    <number:time-style style:name="N159">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+    </number:time-style>
+    <number:time-style style:name="N152">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:time-style style:name="N141" number:truncate-on-overflow="false">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N140">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N138P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N138P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N138P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:text-style style:name="N138">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N138P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N138P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N138P2"/>
-    </number:text-style>
-    <number:currency-style style:name="N137P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N137P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N137P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N137">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N137P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N137P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N137P2"/>
-    </number:text-style>
-    <number:number-style style:name="N136P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N136P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N136P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N136">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N136P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N136P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N136P2"/>
-    </number:text-style>
-    <number:number-style style:name="N135P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N135">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N135P0"/>
-    </number:number-style>
-    <number:number-style style:name="N134P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N134">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N134P0"/>
-    </number:number-style>
-    <number:currency-style style:name="N121P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N121">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N122P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N122">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N122P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N123P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N123">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N123P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N124P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N124">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N124P0"/>
-    </number:currency-style>
-    <number:date-style style:name="N125">
-      <number:month/>
-      <number:text>/</number:text>
-      <number:day/>
-      <number:text>/</number:text>
-      <number:year number:style="long"/>
-    </number:date-style>
-    <number:date-style style:name="N126">
-      <number:day/>
-      <number:text>-</number:text>
-      <number:month number:textual="true"/>
-      <number:text>-</number:text>
-      <number:year/>
-    </number:date-style>
-    <number:date-style style:name="N127">
-      <number:day/>
-      <number:text>-</number:text>
-      <number:month number:textual="true"/>
-    </number:date-style>
-    <number:date-style style:name="N128">
-      <number:month number:textual="true"/>
-      <number:text>-</number:text>
-      <number:year/>
-    </number:date-style>
-    <number:time-style style:name="N129">
+    <number:time-style style:name="N151">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N130">
+    <number:number-style style:name="N150">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
+    <number:date-style style:name="N149">
+      <number:month number:textual="true"/>
+      <number:text>-</number:text>
+      <number:year/>
+    </number:date-style>
+    <number:percentage-style style:name="N148">
+      <number:number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1"/>
+      <number:text>%</number:text>
+    </number:percentage-style>
+    <number:date-style style:name="N147">
+      <number:day/>
+      <number:text>-</number:text>
+      <number:month number:textual="true"/>
+    </number:date-style>
+    <number:time-style style:name="N153">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
@@ -6752,19 +6533,26 @@
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N131">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N132">
+    <number:currency-style style:name="N137P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N137">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N137P0"/>
+    </number:currency-style>
+    <number:time-style style:name="N154" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:date-style style:name="N133">
+    <number:date-style style:name="N125">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
@@ -6775,6 +6563,182 @@
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:date-style>
+    <number:number-style style:name="N138">
+      <number:text>$</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+    </number:number-style>
+    <number:time-style style:name="N126">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:date-style style:name="N139">
+      <number:day/>
+      <number:text>-</number:text>
+      <number:month number:textual="true"/>
+      <number:text>-</number:text>
+      <number:year/>
+    </number:date-style>
+    <number:date-style style:name="N127">
+      <number:month/>
+      <number:text>/</number:text>
+      <number:day/>
+      <number:text>/</number:text>
+      <number:year number:style="long"/>
+    </number:date-style>
+    <number:number-style style:name="N158P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N158P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N158P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:number-style>
+    <number:text-style style:name="N158">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N158P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N158P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N158P2"/>
+    </number:text-style>
+    <number:currency-style style:name="N129P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N129">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N129P0"/>
+    </number:currency-style>
+    <number:number-style style:name="N142P0" style:volatile="true">
+      <number:text> $</number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N142P1" style:volatile="true">
+      <number:text> $</number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N142P2" style:volatile="true">
+      <number:text> $</number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:text-style style:name="N142">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N142P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N142P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N142P2"/>
+    </number:text-style>
+    <number:time-style style:name="N160">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:currency-style style:name="N131P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N131">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N131P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N132P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N132">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N132P0"/>
+    </number:currency-style>
+    <number:number-style style:name="N136P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N136P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N136P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:text-style style:name="N136">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N136P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N136P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N136P2"/>
+    </number:text-style>
+    <number:currency-style style:name="N146P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N146P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N146P2" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N146">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N146P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N146P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N146P2"/>
+    </number:text-style>
     <style:style style:name="Default" style:family="table-cell"/>
     <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:color="#000000" fo:font-size="24pt" fo:font-style="normal" fo:font-weight="bold" style:font-size-asian="24pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-size-complex="24pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
@@ -6833,7 +6797,7 @@
     <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-style-complex="italic" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="Excel_20_Built-in_20_Currency" style:display-name="Excel Built-in Currency" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N139"/>
+    <style:style style:name="Excel_20_Built-in_20_Currency" style:display-name="Excel Built-in Currency" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N124"/>
   </office:styles>
   <office:automatic-styles>
     <style:page-layout style:name="Mpm1">

</xml_diff>